<commit_message>
Work with RBTree was done without debug
</commit_message>
<xml_diff>
--- a/CW_ThoughtsOutLoud/Documents/Книга1.xlsx
+++ b/CW_ThoughtsOutLoud/Documents/Книга1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fosti\source\repos\Fostiriy\University\CW_ThoughtsOutLoud\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C493DA7-070C-4863-9C7A-E48E15285A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DC161F-7F29-4AB8-A881-EDD682CCD597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{A80E80F6-15F0-443C-827D-E94124B27E61}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Имя аудиозаписи</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Лекция 1</t>
-  </si>
-  <si>
-    <t>Лекция 2</t>
   </si>
   <si>
     <t>Запись 29-05</t>
@@ -458,7 +455,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,7 +489,7 @@
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
         <v>44170</v>
@@ -503,7 +500,7 @@
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>43180</v>
@@ -514,7 +511,7 @@
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>44345</v>
@@ -525,7 +522,7 @@
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>43500</v>
@@ -536,7 +533,7 @@
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>44177</v>
@@ -547,7 +544,7 @@
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>44200</v>
@@ -558,7 +555,7 @@
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>44313</v>

</xml_diff>